<commit_message>
Guest table is success FB is not success
start new activity
</commit_message>
<xml_diff>
--- a/Draft DB.xlsx
+++ b/Draft DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/napatcholthaipanich/AndroidStudioProjects/ICTWordGuessingGames/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2496E9-33B9-014E-B471-290AC7622B63}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351DC351-2CE2-8843-93C0-7CDDD4601297}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14000" xr2:uid="{CB17A2FE-73C8-A74E-807E-543997934FC2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{CB17A2FE-73C8-A74E-807E-543997934FC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,15 +51,9 @@
     <t>token</t>
   </si>
   <si>
-    <t>table: category</t>
-  </si>
-  <si>
     <t>cat</t>
   </si>
   <si>
-    <t>table: level</t>
-  </si>
-  <si>
     <t>Q</t>
   </si>
   <si>
@@ -88,6 +82,12 @@
   </si>
   <si>
     <t>F_ID</t>
+  </si>
+  <si>
+    <t>table: Category</t>
+  </si>
+  <si>
+    <t>table: Level</t>
   </si>
 </sst>
 </file>
@@ -139,15 +139,15 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,188 +465,188 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="E7" sqref="E7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="3"/>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="2"/>
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="E2" s="2" t="s">
+      <c r="C2" s="3"/>
+      <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="E3" s="2" t="s">
+      <c r="C3" s="3"/>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="2"/>
+      <c r="E7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="E8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="E10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="C12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="C13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="C14" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="E4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="E5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="3"/>
-      <c r="E7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="2" t="s">
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="C15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4">
+      <c r="C17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="3:4">
+      <c r="C18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="E8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="E9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="E10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="5" t="s">
+    </row>
+    <row r="19" spans="3:4">
+      <c r="C19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="C12" s="1" t="s">
+    <row r="20" spans="3:4">
+      <c r="C20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="C13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="C14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="C15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4">
-      <c r="C17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="3:4">
-      <c r="C18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4">
-      <c r="C19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="3:4">
-      <c r="C20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>15</v>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="C17:D17"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C17:D17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>